<commit_message>
Starting to rename columns
</commit_message>
<xml_diff>
--- a/Math Courses Taken by MATH.1 Placements.xlsx
+++ b/Math Courses Taken by MATH.1 Placements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Desktop\Monmouth\SP_2022\MA321\client_datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Desktop\Monmouth\SP_2022\MA321\MA321-RStudio\MA321-Dr.Coyle-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3B6B67-D128-4105-AC9C-A57263B0145B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880A279B-CBC1-4921-9AB3-93DFEB143AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2679" uniqueCount="138">
   <si>
     <t>Term</t>
   </si>
@@ -535,57 +535,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -846,13 +795,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -866,6 +808,64 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -893,7 +893,7 @@
     <tableColumn id="4" xr3:uid="{B28FDA2D-3465-4D15-BBE6-FF40E77E9AA5}" name="Section Name "/>
     <tableColumn id="5" xr3:uid="{602DE3F2-B5EA-416A-AB8B-216838203836}" name="Current Status"/>
     <tableColumn id="6" xr3:uid="{20231E54-F0EA-4B23-A3EF-772935288941}" name="Verif Grade"/>
-    <tableColumn id="7" xr3:uid="{7BE387D8-61D9-473B-B855-6BA1670EC68C}" name="Actual Grade" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{7BE387D8-61D9-473B-B855-6BA1670EC68C}" name="Actual Grade" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Verif Grade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -902,16 +902,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D072FE4D-0121-4451-A56C-299F0140DF42}" name="Table2" displayName="Table2" ref="A1:G90" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D072FE4D-0121-4451-A56C-299F0140DF42}" name="Table2" displayName="Table2" ref="A1:G90" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A1:G90" xr:uid="{D072FE4D-0121-4451-A56C-299F0140DF42}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8A6CF022-2FC0-482A-AA99-B08CC98B5E99}" name="ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{75319601-D046-446F-8768-3BDA663F2CDC}" name="Term" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C516D1C7-0E42-4E33-9349-9395A2EFBC9D}" name="Course" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{31E33CF5-70F3-468A-A1EC-8E40A0694A52}" name="Section" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{C4DC823A-17D0-4795-89A8-A443CD1BB64F}" name="Current Status" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D9F294B9-403B-44DD-81A4-621471758D70}" name="Verif Grade" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{CD19EDE0-E522-42A4-A5BF-821B02A0D215}" name="Actual Grade" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{8A6CF022-2FC0-482A-AA99-B08CC98B5E99}" name="ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{75319601-D046-446F-8768-3BDA663F2CDC}" name="Term" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C516D1C7-0E42-4E33-9349-9395A2EFBC9D}" name="Course" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{31E33CF5-70F3-468A-A1EC-8E40A0694A52}" name="Section" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{C4DC823A-17D0-4795-89A8-A443CD1BB64F}" name="Current Status" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D9F294B9-403B-44DD-81A4-621471758D70}" name="Verif Grade" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CD19EDE0-E522-42A4-A5BF-821B02A0D215}" name="Actual Grade" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G489"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C304" sqref="C304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1273,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f>IF(F2="R","R",F2)</f>
         <v>F</v>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
         <v>65</v>
       </c>
       <c r="G3" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" ref="G3:G6" si="0">IF(F3="R","R",F3)</f>
         <v>C-</v>
       </c>
     </row>
@@ -1321,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="G4" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
     </row>
@@ -1345,7 +1345,7 @@
         <v>14</v>
       </c>
       <c r="G5" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="0"/>
         <v>C+</v>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
         <v>103</v>
       </c>
       <c r="G6" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="0"/>
         <v>D-</v>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" ref="G8:G13" si="1">IF(F8="R","R",F8)</f>
         <v>A-</v>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
         <v>23</v>
       </c>
       <c r="G9" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="1"/>
         <v>C</v>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
         <v>13</v>
       </c>
       <c r="G10" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="1"/>
         <v>A</v>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
         <v>9</v>
       </c>
       <c r="G11" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="1"/>
         <v>B</v>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
         <v>54</v>
       </c>
       <c r="G12" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="1"/>
         <v>P</v>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
         <v>14</v>
       </c>
       <c r="G13" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="1"/>
         <v>C+</v>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
         <v>13</v>
       </c>
       <c r="G16" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" ref="G16:G37" si="2">IF(F16="R","R",F16)</f>
         <v>A</v>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
         <v>9</v>
       </c>
       <c r="G17" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
         <v>23</v>
       </c>
       <c r="G18" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
         <v>68</v>
       </c>
       <c r="G19" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>D+</v>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
         <v>9</v>
       </c>
       <c r="G20" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -1711,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="G21" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -1735,7 +1735,7 @@
         <v>27</v>
       </c>
       <c r="G22" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
         <v>27</v>
       </c>
       <c r="G23" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -1783,7 +1783,7 @@
         <v>27</v>
       </c>
       <c r="G24" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
         <v>27</v>
       </c>
       <c r="G25" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
         <v>13</v>
       </c>
       <c r="G26" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
         <v>9</v>
       </c>
       <c r="G27" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
         <v>65</v>
       </c>
       <c r="G28" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>C-</v>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
         <v>9</v>
       </c>
       <c r="G29" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
         <v>23</v>
       </c>
       <c r="G30" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
         <v>68</v>
       </c>
       <c r="G31" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>D+</v>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
         <v>13</v>
       </c>
       <c r="G32" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
         <v>13</v>
       </c>
       <c r="G33" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -2023,7 +2023,7 @@
         <v>27</v>
       </c>
       <c r="G34" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
         <v>17</v>
       </c>
       <c r="G35" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>B+</v>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
         <v>9</v>
       </c>
       <c r="G36" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -2095,7 +2095,7 @@
         <v>68</v>
       </c>
       <c r="G37" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="2"/>
         <v>D+</v>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
         <v>13</v>
       </c>
       <c r="G39" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" ref="G39:G56" si="3">IF(F39="R","R",F39)</f>
         <v>A</v>
       </c>
     </row>
@@ -2161,7 +2161,7 @@
         <v>23</v>
       </c>
       <c r="G40" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>C</v>
       </c>
     </row>
@@ -2185,7 +2185,7 @@
         <v>13</v>
       </c>
       <c r="G41" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>A</v>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
         <v>23</v>
       </c>
       <c r="G42" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>C</v>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
         <v>13</v>
       </c>
       <c r="G43" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>A</v>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
         <v>13</v>
       </c>
       <c r="G44" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>A</v>
       </c>
     </row>
@@ -2281,7 +2281,7 @@
         <v>37</v>
       </c>
       <c r="G45" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>B-</v>
       </c>
     </row>
@@ -2305,7 +2305,7 @@
         <v>9</v>
       </c>
       <c r="G46" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>B</v>
       </c>
     </row>
@@ -2329,7 +2329,7 @@
         <v>68</v>
       </c>
       <c r="G47" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>D+</v>
       </c>
     </row>
@@ -2353,7 +2353,7 @@
         <v>23</v>
       </c>
       <c r="G48" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>C</v>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
         <v>13</v>
       </c>
       <c r="G49" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>A</v>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
         <v>65</v>
       </c>
       <c r="G50" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>C-</v>
       </c>
     </row>
@@ -2425,7 +2425,7 @@
         <v>23</v>
       </c>
       <c r="G51" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>C</v>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
         <v>17</v>
       </c>
       <c r="G52" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>B+</v>
       </c>
     </row>
@@ -2473,7 +2473,7 @@
         <v>37</v>
       </c>
       <c r="G53" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>B-</v>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
         <v>65</v>
       </c>
       <c r="G54" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>C-</v>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
         <v>27</v>
       </c>
       <c r="G55" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>A-</v>
       </c>
     </row>
@@ -2545,7 +2545,7 @@
         <v>13</v>
       </c>
       <c r="G56" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="3"/>
         <v>A</v>
       </c>
     </row>
@@ -2587,7 +2587,7 @@
         <v>37</v>
       </c>
       <c r="G58" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" ref="G58:G118" si="4">IF(F58="R","R",F58)</f>
         <v>B-</v>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
         <v>65</v>
       </c>
       <c r="G59" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>C-</v>
       </c>
     </row>
@@ -2635,7 +2635,7 @@
         <v>65</v>
       </c>
       <c r="G60" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>C-</v>
       </c>
     </row>
@@ -2659,7 +2659,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
         <v>13</v>
       </c>
       <c r="G62" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
         <v>68</v>
       </c>
       <c r="G63" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>D+</v>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
         <v>23</v>
       </c>
       <c r="G64" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
@@ -2755,7 +2755,7 @@
         <v>37</v>
       </c>
       <c r="G65" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -2779,7 +2779,7 @@
         <v>9</v>
       </c>
       <c r="G66" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -2803,7 +2803,7 @@
         <v>68</v>
       </c>
       <c r="G67" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>D+</v>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
         <v>35</v>
       </c>
       <c r="G68" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
         <v>13</v>
       </c>
       <c r="G69" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2875,7 +2875,7 @@
         <v>13</v>
       </c>
       <c r="G70" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2923,7 +2923,7 @@
         <v>62</v>
       </c>
       <c r="G72" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
         <v>13</v>
       </c>
       <c r="G73" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2971,7 +2971,7 @@
         <v>13</v>
       </c>
       <c r="G74" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -2995,7 +2995,7 @@
         <v>9</v>
       </c>
       <c r="G75" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3019,7 +3019,7 @@
         <v>37</v>
       </c>
       <c r="G76" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -3043,7 +3043,7 @@
         <v>13</v>
       </c>
       <c r="G77" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
         <v>13</v>
       </c>
       <c r="G78" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
         <v>17</v>
       </c>
       <c r="G79" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3115,7 +3115,7 @@
         <v>13</v>
       </c>
       <c r="G80" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3139,7 +3139,7 @@
         <v>17</v>
       </c>
       <c r="G81" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3163,7 +3163,7 @@
         <v>9</v>
       </c>
       <c r="G82" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3187,7 +3187,7 @@
         <v>37</v>
       </c>
       <c r="G83" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -3211,7 +3211,7 @@
         <v>13</v>
       </c>
       <c r="G84" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3235,7 +3235,7 @@
         <v>65</v>
       </c>
       <c r="G85" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>C-</v>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
         <v>62</v>
       </c>
       <c r="G86" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
@@ -3283,7 +3283,7 @@
         <v>9</v>
       </c>
       <c r="G87" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3307,7 +3307,7 @@
         <v>13</v>
       </c>
       <c r="G88" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3331,7 +3331,7 @@
         <v>17</v>
       </c>
       <c r="G89" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
         <v>27</v>
       </c>
       <c r="G90" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
@@ -3379,7 +3379,7 @@
         <v>17</v>
       </c>
       <c r="G91" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3403,7 +3403,7 @@
         <v>17</v>
       </c>
       <c r="G92" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
         <v>9</v>
       </c>
       <c r="G93" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3451,7 +3451,7 @@
         <v>13</v>
       </c>
       <c r="G94" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3475,7 +3475,7 @@
         <v>37</v>
       </c>
       <c r="G95" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -3499,7 +3499,7 @@
         <v>17</v>
       </c>
       <c r="G96" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3523,7 +3523,7 @@
         <v>54</v>
       </c>
       <c r="G97" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>P</v>
       </c>
     </row>
@@ -3547,7 +3547,7 @@
         <v>37</v>
       </c>
       <c r="G98" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -3571,7 +3571,7 @@
         <v>37</v>
       </c>
       <c r="G99" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
         <v>13</v>
       </c>
       <c r="G100" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
         <v>54</v>
       </c>
       <c r="G101" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>P</v>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
         <v>27</v>
       </c>
       <c r="G102" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
@@ -3667,7 +3667,7 @@
         <v>9</v>
       </c>
       <c r="G103" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3691,7 +3691,7 @@
         <v>9</v>
       </c>
       <c r="G104" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
         <v>9</v>
       </c>
       <c r="G105" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3739,7 +3739,7 @@
         <v>27</v>
       </c>
       <c r="G106" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
@@ -3763,7 +3763,7 @@
         <v>17</v>
       </c>
       <c r="G107" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
         <v>13</v>
       </c>
       <c r="G108" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
@@ -3811,7 +3811,7 @@
         <v>27</v>
       </c>
       <c r="G109" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
@@ -3835,7 +3835,7 @@
         <v>9</v>
       </c>
       <c r="G110" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3859,7 +3859,7 @@
         <v>23</v>
       </c>
       <c r="G111" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
         <v>17</v>
       </c>
       <c r="G112" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3907,7 +3907,7 @@
         <v>17</v>
       </c>
       <c r="G113" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
@@ -3931,7 +3931,7 @@
         <v>54</v>
       </c>
       <c r="G114" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>P</v>
       </c>
     </row>
@@ -3955,7 +3955,7 @@
         <v>9</v>
       </c>
       <c r="G115" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
@@ -3979,7 +3979,7 @@
         <v>27</v>
       </c>
       <c r="G116" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
@@ -4003,7 +4003,7 @@
         <v>23</v>
       </c>
       <c r="G117" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
@@ -4027,7 +4027,7 @@
         <v>37</v>
       </c>
       <c r="G118" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
@@ -4072,7 +4072,7 @@
         <v>65</v>
       </c>
       <c r="G120" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" ref="G120:G135" si="5">IF(F120="R","R",F120)</f>
         <v>C-</v>
       </c>
     </row>
@@ -4095,8 +4095,9 @@
       <c r="F121" t="s">
         <v>73</v>
       </c>
-      <c r="G121" t="s">
-        <v>62</v>
+      <c r="G121" t="str">
+        <f>IF(F121="R","F",F121)</f>
+        <v>F</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4119,7 +4120,7 @@
         <v>65</v>
       </c>
       <c r="G122" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>C-</v>
       </c>
     </row>
@@ -4143,7 +4144,7 @@
         <v>13</v>
       </c>
       <c r="G123" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
@@ -4167,7 +4168,7 @@
         <v>13</v>
       </c>
       <c r="G124" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
@@ -4191,7 +4192,7 @@
         <v>17</v>
       </c>
       <c r="G125" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>B+</v>
       </c>
     </row>
@@ -4215,7 +4216,7 @@
         <v>17</v>
       </c>
       <c r="G126" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>B+</v>
       </c>
     </row>
@@ -4239,7 +4240,7 @@
         <v>27</v>
       </c>
       <c r="G127" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>A-</v>
       </c>
     </row>
@@ -4263,7 +4264,7 @@
         <v>9</v>
       </c>
       <c r="G128" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>B</v>
       </c>
     </row>
@@ -4287,7 +4288,7 @@
         <v>17</v>
       </c>
       <c r="G129" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>B+</v>
       </c>
     </row>
@@ -4311,7 +4312,7 @@
         <v>81</v>
       </c>
       <c r="G130" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>D</v>
       </c>
     </row>
@@ -4335,7 +4336,7 @@
         <v>23</v>
       </c>
       <c r="G131" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>C</v>
       </c>
     </row>
@@ -4359,7 +4360,7 @@
         <v>9</v>
       </c>
       <c r="G132" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>B</v>
       </c>
     </row>
@@ -4382,8 +4383,9 @@
       <c r="F133" t="s">
         <v>73</v>
       </c>
-      <c r="G133" t="s">
-        <v>62</v>
+      <c r="G133" t="str">
+        <f>IF(F133="R","F",F133)</f>
+        <v>F</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4406,7 +4408,7 @@
         <v>65</v>
       </c>
       <c r="G134" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>C-</v>
       </c>
     </row>
@@ -4430,7 +4432,7 @@
         <v>17</v>
       </c>
       <c r="G135" t="str">
-        <f>Table1[[#This Row],[Verif Grade]]</f>
+        <f t="shared" si="5"/>
         <v>B+</v>
       </c>
     </row>
@@ -8062,8 +8064,9 @@
       <c r="F288" t="s">
         <v>73</v>
       </c>
-      <c r="G288" t="s">
-        <v>62</v>
+      <c r="G288" t="str">
+        <f>IF(F288="R","F",F288)</f>
+        <v>F</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
@@ -8988,8 +8991,9 @@
       <c r="F328" t="s">
         <v>73</v>
       </c>
-      <c r="G328" t="s">
-        <v>62</v>
+      <c r="G328" t="str">
+        <f>IF(F328="R","F",F328)</f>
+        <v>F</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
@@ -9428,8 +9432,9 @@
       <c r="F348" t="s">
         <v>73</v>
       </c>
-      <c r="G348" t="s">
-        <v>62</v>
+      <c r="G348" t="str">
+        <f>IF(F348="R","F",F348)</f>
+        <v>F</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -9589,8 +9594,9 @@
       <c r="F355" t="s">
         <v>73</v>
       </c>
-      <c r="G355" t="s">
-        <v>62</v>
+      <c r="G355" t="str">
+        <f>IF(F355="R","F",F355)</f>
+        <v>F</v>
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
@@ -12563,7 +12569,7 @@
   <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>